<commit_message>
refactor: invoice & invoice_items scopes / code simplification
</commit_message>
<xml_diff>
--- a/db/data/export/export_providers.xlsx
+++ b/db/data/export/export_providers.xlsx
@@ -399,28 +399,28 @@
     </row>
     <row r="2" spans="1:8" customFormat="false">
       <c r="A2" s="0">
-        <v>67.1316</v>
+        <v>201.39480000000006</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>67.1316</v>
+        <v>201.39480000000006</v>
       </c>
       <c r="D2" s="0">
-        <v>39.1012</v>
+        <v>117.3036</v>
       </c>
       <c r="E2" s="0">
-        <v>28.0304</v>
+        <v>84.0912</v>
       </c>
       <c r="F2" s="0">
-        <v>2.35</v>
+        <v>7.050000000000001</v>
       </c>
       <c r="G2" s="0">
-        <v>64.7816</v>
+        <v>194.34480000000005</v>
       </c>
       <c r="H2" s="0">
-        <v>12.496295000000002</v>
+        <v>37.488884999999996</v>
       </c>
     </row>
   </sheetData>
@@ -459,28 +459,28 @@
     </row>
     <row r="2" spans="1:8" customFormat="false">
       <c r="A2" s="0">
-        <v>298.72500000000014</v>
+        <v>896.1749999999996</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>298.72500000000014</v>
+        <v>896.1749999999996</v>
       </c>
       <c r="D2" s="0">
-        <v>210.225</v>
+        <v>646.1149999999998</v>
       </c>
       <c r="E2" s="0">
-        <v>88.49999999999999</v>
+        <v>250.06000000000003</v>
       </c>
       <c r="F2" s="0">
-        <v>15.44</v>
+        <v>46.32</v>
       </c>
       <c r="G2" s="0">
-        <v>283.28500000000014</v>
+        <v>849.8549999999998</v>
       </c>
       <c r="H2" s="0">
-        <v>56.86974999999999</v>
+        <v>170.16225000000014</v>
       </c>
     </row>
   </sheetData>
@@ -579,28 +579,28 @@
     </row>
     <row r="2" spans="1:8" customFormat="false">
       <c r="A2" s="0">
-        <v>408.60400000000004</v>
+        <v>1225.812</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>408.60400000000004</v>
+        <v>1225.812</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
       </c>
       <c r="E2" s="0">
-        <v>408.60400000000004</v>
+        <v>1225.812</v>
       </c>
       <c r="F2" s="0">
         <v>0</v>
       </c>
       <c r="G2" s="0">
-        <v>408.60400000000004</v>
+        <v>1225.812</v>
       </c>
       <c r="H2" s="0">
-        <v>81.7208</v>
+        <v>245.1624</v>
       </c>
     </row>
   </sheetData>
@@ -639,28 +639,28 @@
     </row>
     <row r="2" spans="1:8" customFormat="false">
       <c r="A2" s="0">
-        <v>67.016</v>
+        <v>201.04800000000003</v>
       </c>
       <c r="B2" s="0">
-        <v>40.8909</v>
+        <v>122.6727</v>
       </c>
       <c r="C2" s="0">
-        <v>26.1251</v>
+        <v>78.37530000000001</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
       </c>
       <c r="E2" s="0">
-        <v>67.016</v>
+        <v>201.04800000000003</v>
       </c>
       <c r="F2" s="0">
         <v>0</v>
       </c>
       <c r="G2" s="0">
-        <v>67.016</v>
+        <v>201.04800000000003</v>
       </c>
       <c r="H2" s="0">
-        <v>13.403199999999998</v>
+        <v>40.20960000000002</v>
       </c>
     </row>
   </sheetData>
@@ -699,28 +699,28 @@
     </row>
     <row r="2" spans="1:8" customFormat="false">
       <c r="A2" s="0">
-        <v>51.839999999999996</v>
+        <v>155.52</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>51.839999999999996</v>
+        <v>155.52</v>
       </c>
       <c r="D2" s="0">
-        <v>0</v>
+        <v>37.14</v>
       </c>
       <c r="E2" s="0">
-        <v>51.839999999999996</v>
+        <v>118.37999999999998</v>
       </c>
       <c r="F2" s="0">
         <v>0</v>
       </c>
       <c r="G2" s="0">
-        <v>51.839999999999996</v>
+        <v>155.52</v>
       </c>
       <c r="H2" s="0">
-        <v>10.367999999999999</v>
+        <v>29.247000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -759,28 +759,28 @@
     </row>
     <row r="2" spans="1:8" customFormat="false">
       <c r="A2" s="0">
-        <v>3367.5099999999998</v>
+        <v>10102.530000000006</v>
       </c>
       <c r="B2" s="0">
-        <v>873.9099999999996</v>
+        <v>2621.7299999999996</v>
       </c>
       <c r="C2" s="0">
-        <v>2493.5999999999995</v>
+        <v>7480.800000000001</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
       </c>
       <c r="E2" s="0">
-        <v>3367.5099999999998</v>
+        <v>10102.530000000006</v>
       </c>
       <c r="F2" s="0">
-        <v>4.09</v>
+        <v>12.27</v>
       </c>
       <c r="G2" s="0">
-        <v>3363.4199999999996</v>
+        <v>10090.260000000006</v>
       </c>
       <c r="H2" s="0">
-        <v>673.5019999999998</v>
+        <v>2020.505999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>